<commit_message>
Added first test case; updated requirements table
</commit_message>
<xml_diff>
--- a/Documentation/Requirements Table Rev3.xlsx
+++ b/Documentation/Requirements Table Rev3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Randu\Google Drive\Classwork\CSE3310\FundamentalsPokerGame\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbie\Documents\GitHub\FundamentalsPokerGame\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96982E10-3492-4E1F-A7B0-411AF5566A87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F546A179-F3F0-44FB-9F91-545AE45B8245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17025" yWindow="0" windowWidth="17025" windowHeight="21000" xr2:uid="{9F63A9F9-7C5B-4B89-AA9A-0F55721D7DEB}"/>
+    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" xr2:uid="{9F63A9F9-7C5B-4B89-AA9A-0F55721D7DEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="110">
   <si>
     <t>REQID</t>
   </si>
@@ -251,32 +251,7 @@
     <t>A second instance of the dealer application will fail to open on the same port</t>
   </si>
   <si>
-    <t>Gameplay will not start with fewer than two player processes
-The dealer will not accept a sixth player process until an existing player has left the game</t>
-  </si>
-  <si>
     <t>Each suit shall consist of cards Ace, 2, 3, 4, 5, 6, 7 ,8 ,9, 10, Jack, Queen, King</t>
-  </si>
-  <si>
-    <t>Verify the initial ante is equal to the number of player processes</t>
-  </si>
-  <si>
-    <t>Test that buttons are active for player in turn and inactive for players out of turn</t>
-  </si>
-  <si>
-    <t>If prize pot &gt; ante, check button is inactive for all players</t>
-  </si>
-  <si>
-    <t>Verify the bet value token after a bet is placed</t>
-  </si>
-  <si>
-    <t>Set a must bet flag for all other players when a player increases the bet amount</t>
-  </si>
-  <si>
-    <t>Verify the bet value token after the bet is raised</t>
-  </si>
-  <si>
-    <t>Verify that the player bet amount changed to match the bet amount</t>
   </si>
   <si>
     <t>Verify all buttons are inactive for folded player</t>
@@ -398,6 +373,9 @@
   </si>
   <si>
     <t>Game::discard_pile</t>
+  </si>
+  <si>
+    <t>Test case 1</t>
   </si>
 </sst>
 </file>
@@ -1133,9 +1111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44B577E-68CC-4E7A-8A29-E66A7405A411}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1192,10 +1168,10 @@
         <v>71</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="H2" s="8"/>
     </row>
@@ -1214,14 +1190,14 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1235,13 +1211,13 @@
         <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H4" s="8"/>
     </row>
@@ -1260,10 +1236,10 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H5" s="8"/>
     </row>
@@ -1280,12 +1256,14 @@
       <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F6" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="H6" s="8"/>
     </row>
@@ -1304,10 +1282,10 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H7" s="8"/>
     </row>
@@ -1326,10 +1304,10 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H8" s="8"/>
     </row>
@@ -1344,14 +1322,14 @@
         <v>63</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H9" s="8"/>
     </row>
@@ -1370,10 +1348,10 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H10" s="8"/>
     </row>
@@ -1388,14 +1366,14 @@
         <v>63</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H11" s="8"/>
     </row>
@@ -1414,10 +1392,10 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H12" s="8"/>
     </row>
@@ -1436,10 +1414,10 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H13" s="8"/>
     </row>
@@ -1458,11 +1436,11 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1480,11 +1458,11 @@
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1502,11 +1480,11 @@
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1524,11 +1502,11 @@
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1542,17 +1520,19 @@
         <v>64</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E18" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1568,12 +1548,14 @@
       <c r="D19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F19" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H19" s="8"/>
     </row>
@@ -1591,13 +1573,13 @@
         <v>24</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="H20" s="8"/>
     </row>
@@ -1614,12 +1596,14 @@
       <c r="D21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F21" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="H21" s="8"/>
     </row>
@@ -1637,13 +1621,13 @@
         <v>21</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="H22" s="8"/>
     </row>
@@ -1662,10 +1646,10 @@
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="H23" s="8"/>
     </row>
@@ -1683,13 +1667,13 @@
         <v>23</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="H24" s="8"/>
     </row>
@@ -1708,14 +1692,14 @@
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>10.050000000000001</v>
       </c>
@@ -1728,12 +1712,14 @@
       <c r="D26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F26" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="H26" s="8"/>
     </row>
@@ -1751,13 +1737,13 @@
         <v>30</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H27" s="8"/>
     </row>
@@ -1775,13 +1761,13 @@
         <v>31</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H28" s="8"/>
     </row>
@@ -1799,13 +1785,13 @@
         <v>28</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H29" s="8"/>
     </row>
@@ -1823,13 +1809,13 @@
         <v>29</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H30" s="8"/>
     </row>
@@ -1846,12 +1832,14 @@
       <c r="D31" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F31" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H31" s="8"/>
     </row>
@@ -1869,13 +1857,13 @@
         <v>32</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H32" s="8"/>
     </row>
@@ -1894,10 +1882,10 @@
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H33" s="8"/>
     </row>
@@ -1915,13 +1903,13 @@
         <v>34</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H34" s="8"/>
     </row>
@@ -1940,10 +1928,10 @@
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="H35" s="8"/>
     </row>
@@ -1960,12 +1948,14 @@
       <c r="D36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E36" s="3"/>
+      <c r="E36" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F36" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="H36" s="8"/>
     </row>
@@ -1982,12 +1972,14 @@
       <c r="D37" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="3"/>
+      <c r="E37" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F37" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="H37" s="8"/>
     </row>
@@ -2004,12 +1996,14 @@
       <c r="D38" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="3"/>
+      <c r="E38" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F38" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H38" s="8"/>
     </row>
@@ -2026,9 +2020,11 @@
       <c r="D39" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="3"/>
+      <c r="E39" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F39" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="8"/>
@@ -2046,12 +2042,14 @@
       <c r="D40" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F40" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H40" s="8"/>
     </row>
@@ -2068,12 +2066,14 @@
       <c r="D41" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F41" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H41" s="8"/>
     </row>
@@ -2092,10 +2092,10 @@
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H42" s="8"/>
     </row>
@@ -2114,10 +2114,10 @@
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H43" s="8"/>
     </row>
@@ -2136,10 +2136,10 @@
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H44" s="8"/>
     </row>
@@ -2158,10 +2158,10 @@
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H45" s="8"/>
     </row>
@@ -2180,10 +2180,10 @@
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H46" s="8"/>
     </row>
@@ -2202,10 +2202,10 @@
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H47" s="8"/>
     </row>
@@ -2224,10 +2224,10 @@
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H48" s="8"/>
     </row>
@@ -2246,10 +2246,10 @@
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H49" s="8"/>
     </row>
@@ -2268,10 +2268,10 @@
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H50" s="8"/>
     </row>
@@ -2290,10 +2290,10 @@
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H51" s="8"/>
     </row>
@@ -2312,10 +2312,10 @@
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H52" s="8"/>
     </row>
@@ -2334,10 +2334,10 @@
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="H53" s="8"/>
     </row>
@@ -2356,10 +2356,10 @@
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H54" s="8"/>
     </row>
@@ -2378,10 +2378,10 @@
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H55" s="8"/>
     </row>
@@ -2400,10 +2400,10 @@
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H56" s="8"/>
     </row>
@@ -2422,10 +2422,10 @@
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H57" s="8"/>
     </row>
@@ -2444,10 +2444,10 @@
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H58" s="8"/>
     </row>
@@ -2466,10 +2466,10 @@
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H59" s="8"/>
     </row>
@@ -2488,10 +2488,10 @@
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H60" s="8"/>
     </row>
@@ -2510,10 +2510,10 @@
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H61" s="8"/>
     </row>
@@ -2530,10 +2530,10 @@
       </c>
       <c r="E62" s="15"/>
       <c r="F62" s="15" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H62" s="16"/>
     </row>

</xml_diff>

<commit_message>
Define player ties in requirements.
</commit_message>
<xml_diff>
--- a/Documentation/Requirements Table Rev3.xlsx
+++ b/Documentation/Requirements Table Rev3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbie\Documents\GitHub\FundamentalsPokerGame\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Randu\Google Drive\Classwork\CSE3310\FundamentalsPokerGame\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F546A179-F3F0-44FB-9F91-545AE45B8245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5286C91-C321-4434-8521-66C048807872}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" xr2:uid="{9F63A9F9-7C5B-4B89-AA9A-0F55721D7DEB}"/>
+    <workbookView xWindow="17025" yWindow="0" windowWidth="17025" windowHeight="21000" xr2:uid="{9F63A9F9-7C5B-4B89-AA9A-0F55721D7DEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -230,9 +230,6 @@
     <t>Player</t>
   </si>
   <si>
-    <t>***NEED TO DEFINE HOW TO HANDLE TIE***</t>
-  </si>
-  <si>
     <t>Ace can be high (above King) or low (below 2)</t>
   </si>
   <si>
@@ -376,6 +373,9 @@
   </si>
   <si>
     <t>Test case 1</t>
+  </si>
+  <si>
+    <t>Two players have tied. EX: two players have a pair of tens and each have the same card values in descending order. Game shall split the pot between the tied players evenly.</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1111,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44B577E-68CC-4E7A-8A29-E66A7405A411}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1156,7 +1158,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>63</v>
@@ -1165,13 +1167,13 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H2" s="8"/>
     </row>
@@ -1180,7 +1182,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>63</v>
@@ -1190,10 +1192,10 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="H3" s="8"/>
     </row>
@@ -1202,7 +1204,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>63</v>
@@ -1211,13 +1213,13 @@
         <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="8"/>
     </row>
@@ -1226,7 +1228,7 @@
         <v>3.01</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>63</v>
@@ -1236,10 +1238,10 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="8"/>
     </row>
@@ -1248,7 +1250,7 @@
         <v>3.02</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>64</v>
@@ -1257,13 +1259,13 @@
         <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="H6" s="8"/>
     </row>
@@ -1272,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>63</v>
@@ -1282,10 +1284,10 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H7" s="8"/>
     </row>
@@ -1294,7 +1296,7 @@
         <v>4.01</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>63</v>
@@ -1304,10 +1306,10 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H8" s="8"/>
     </row>
@@ -1316,20 +1318,20 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" s="8"/>
     </row>
@@ -1338,20 +1340,20 @@
         <v>4.03</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H10" s="8"/>
     </row>
@@ -1360,20 +1362,20 @@
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H11" s="8"/>
     </row>
@@ -1382,7 +1384,7 @@
         <v>5.01</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>63</v>
@@ -1392,10 +1394,10 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H12" s="8"/>
     </row>
@@ -1404,7 +1406,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>63</v>
@@ -1414,10 +1416,10 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H13" s="8"/>
     </row>
@@ -1426,21 +1428,21 @@
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1448,21 +1450,21 @@
         <v>7.01</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1470,21 +1472,21 @@
         <v>7.02</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1492,21 +1494,21 @@
         <v>7.03</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1514,25 +1516,25 @@
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1540,22 +1542,22 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H19" s="8"/>
     </row>
@@ -1564,7 +1566,7 @@
         <v>9.01</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>63</v>
@@ -1573,13 +1575,13 @@
         <v>24</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H20" s="8"/>
     </row>
@@ -1588,22 +1590,22 @@
         <v>10</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H21" s="8"/>
     </row>
@@ -1612,22 +1614,22 @@
         <v>10.01</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H22" s="8"/>
     </row>
@@ -1636,20 +1638,20 @@
         <v>10.02</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H23" s="8"/>
     </row>
@@ -1658,22 +1660,22 @@
         <v>10.029999999999999</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H24" s="8"/>
     </row>
@@ -1682,20 +1684,20 @@
         <v>10.039999999999999</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H25" s="8"/>
     </row>
@@ -1704,22 +1706,22 @@
         <v>10.050000000000001</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H26" s="8"/>
     </row>
@@ -1728,22 +1730,22 @@
         <v>10.06</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H27" s="8"/>
     </row>
@@ -1752,22 +1754,22 @@
         <v>10.07</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H28" s="8"/>
     </row>
@@ -1776,22 +1778,22 @@
         <v>10.08</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H29" s="8"/>
     </row>
@@ -1800,22 +1802,22 @@
         <v>10.09</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H30" s="8"/>
     </row>
@@ -1824,22 +1826,22 @@
         <v>10.1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H31" s="8"/>
     </row>
@@ -1848,22 +1850,22 @@
         <v>10.11</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H32" s="8"/>
     </row>
@@ -1872,20 +1874,20 @@
         <v>10.119999999999999</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H33" s="8"/>
     </row>
@@ -1894,22 +1896,22 @@
         <v>10.130000000000001</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H34" s="8"/>
     </row>
@@ -1918,20 +1920,20 @@
         <v>10.14</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H35" s="8"/>
     </row>
@@ -1940,22 +1942,22 @@
         <v>11</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H36" s="8"/>
     </row>
@@ -1964,7 +1966,7 @@
         <v>11.01</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>63</v>
@@ -1973,13 +1975,13 @@
         <v>37</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H37" s="8"/>
     </row>
@@ -1988,22 +1990,22 @@
         <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H38" s="8"/>
     </row>
@@ -2012,19 +2014,19 @@
         <v>12.01</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="8"/>
@@ -2034,22 +2036,22 @@
         <v>13</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H40" s="8"/>
     </row>
@@ -2058,22 +2060,22 @@
         <v>13.01</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H41" s="8"/>
     </row>
@@ -2082,7 +2084,7 @@
         <v>13.02</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>63</v>
@@ -2092,10 +2094,10 @@
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H42" s="8"/>
     </row>
@@ -2104,7 +2106,7 @@
         <v>13.03</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>63</v>
@@ -2114,10 +2116,10 @@
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H43" s="8"/>
     </row>
@@ -2126,7 +2128,7 @@
         <v>13.04</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>63</v>
@@ -2136,10 +2138,10 @@
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H44" s="8"/>
     </row>
@@ -2148,7 +2150,7 @@
         <v>13.05</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>63</v>
@@ -2158,10 +2160,10 @@
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H45" s="8"/>
     </row>
@@ -2170,7 +2172,7 @@
         <v>13.06</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>63</v>
@@ -2180,10 +2182,10 @@
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H46" s="8"/>
     </row>
@@ -2192,7 +2194,7 @@
         <v>13.07</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>63</v>
@@ -2202,10 +2204,10 @@
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H47" s="8"/>
     </row>
@@ -2214,7 +2216,7 @@
         <v>13.08</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>63</v>
@@ -2224,10 +2226,10 @@
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H48" s="8"/>
     </row>
@@ -2236,7 +2238,7 @@
         <v>13.09</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>63</v>
@@ -2246,10 +2248,10 @@
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H49" s="8"/>
     </row>
@@ -2258,7 +2260,7 @@
         <v>13.1</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>63</v>
@@ -2268,10 +2270,10 @@
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H50" s="8"/>
     </row>
@@ -2280,7 +2282,7 @@
         <v>13.11</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>63</v>
@@ -2290,10 +2292,10 @@
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H51" s="8"/>
     </row>
@@ -2302,7 +2304,7 @@
         <v>13.12</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>63</v>
@@ -2312,10 +2314,10 @@
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H52" s="8"/>
     </row>
@@ -2324,7 +2326,7 @@
         <v>13.13</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>63</v>
@@ -2334,10 +2336,10 @@
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H53" s="8"/>
     </row>
@@ -2346,7 +2348,7 @@
         <v>13.14</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>63</v>
@@ -2356,10 +2358,10 @@
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H54" s="8"/>
     </row>
@@ -2368,7 +2370,7 @@
         <v>13.15</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>63</v>
@@ -2378,10 +2380,10 @@
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H55" s="8"/>
     </row>
@@ -2390,7 +2392,7 @@
         <v>13.16</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>63</v>
@@ -2400,10 +2402,10 @@
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H56" s="8"/>
     </row>
@@ -2412,7 +2414,7 @@
         <v>13.17</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>63</v>
@@ -2422,10 +2424,10 @@
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H57" s="8"/>
     </row>
@@ -2434,7 +2436,7 @@
         <v>13.18</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>63</v>
@@ -2444,10 +2446,10 @@
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H58" s="8"/>
     </row>
@@ -2456,7 +2458,7 @@
         <v>13.19</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>63</v>
@@ -2466,10 +2468,10 @@
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H59" s="8"/>
     </row>
@@ -2478,7 +2480,7 @@
         <v>13.2</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>63</v>
@@ -2488,10 +2490,10 @@
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H60" s="8"/>
     </row>
@@ -2500,7 +2502,7 @@
         <v>13.21</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>63</v>
@@ -2510,30 +2512,32 @@
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+    <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="14">
+        <v>13.22</v>
+      </c>
       <c r="B62" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>63</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="E62" s="15"/>
       <c r="F62" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H62" s="16"/>
     </row>

</xml_diff>